<commit_message>
fix text cut off
</commit_message>
<xml_diff>
--- a/quotation-template.xlsx
+++ b/quotation-template.xlsx
@@ -138,7 +138,7 @@
     <t>（内訳）</t>
   </si>
   <si>
-    <t xml:space="preserve">               株式会社 クーシー</t>
+    <t xml:space="preserve">            株式会社 クーシー</t>
   </si>
   <si>
     <t xml:space="preserve">                〒150-0011東京都渋谷区東3-16-3 7F</t>
@@ -768,7 +768,7 @@
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -847,7 +847,7 @@
     <xdr:ext cx="1285875" cy="485775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -884,7 +884,7 @@
     <xdr:ext cx="666750" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -921,7 +921,7 @@
     <xdr:ext cx="666750" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -16345,7 +16345,7 @@
       <c r="AB9" s="30"/>
       <c r="AC9" s="30"/>
     </row>
-    <row r="10" ht="13.5" customHeight="1">
+    <row r="10" ht="28.5" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="54" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fix font weight bold
</commit_message>
<xml_diff>
--- a/quotation-template.xlsx
+++ b/quotation-template.xlsx
@@ -551,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -851,6 +851,9 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="21" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="21" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -16483,7 +16486,7 @@
       </c>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
@@ -16516,7 +16519,7 @@
       </c>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="59"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="57"/>
       <c r="G13" s="57"/>
       <c r="H13" s="57"/>
@@ -16586,7 +16589,7 @@
       </c>
       <c r="C15" s="61"/>
       <c r="D15" s="61"/>
-      <c r="E15" s="70"/>
+      <c r="E15" s="110"/>
       <c r="F15" s="61"/>
       <c r="G15" s="61"/>
       <c r="H15" s="61"/>
@@ -16784,7 +16787,7 @@
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="111" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="57"/>
@@ -16799,75 +16802,75 @@
       <c r="L22" s="57"/>
       <c r="M22" s="57"/>
       <c r="N22" s="56"/>
-      <c r="O22" s="111"/>
-      <c r="P22" s="111"/>
-      <c r="Q22" s="111"/>
-      <c r="R22" s="111"/>
-      <c r="S22" s="111"/>
-      <c r="T22" s="111"/>
-      <c r="U22" s="111"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="112"/>
+      <c r="Q22" s="112"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="112"/>
+      <c r="T22" s="112"/>
+      <c r="U22" s="112"/>
       <c r="V22" s="56"/>
-      <c r="W22" s="112"/>
+      <c r="W22" s="113"/>
       <c r="X22" s="56"/>
-      <c r="Y22" s="113"/>
+      <c r="Y22" s="114"/>
       <c r="Z22" s="30"/>
       <c r="AA22" s="30"/>
       <c r="AB22" s="30"/>
       <c r="AC22" s="30"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
-      <c r="A23" s="114"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="114"/>
-      <c r="G23" s="114"/>
-      <c r="H23" s="114"/>
-      <c r="I23" s="114"/>
-      <c r="J23" s="114"/>
-      <c r="K23" s="114"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="114"/>
-      <c r="O23" s="115"/>
-      <c r="P23" s="116"/>
-      <c r="S23" s="116"/>
-      <c r="T23" s="116"/>
-      <c r="V23" s="115"/>
-      <c r="W23" s="115"/>
-      <c r="Z23" s="115"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="115"/>
+      <c r="H23" s="115"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="115"/>
+      <c r="K23" s="115"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
+      <c r="N23" s="115"/>
+      <c r="O23" s="116"/>
+      <c r="P23" s="117"/>
+      <c r="S23" s="117"/>
+      <c r="T23" s="117"/>
+      <c r="V23" s="116"/>
+      <c r="W23" s="116"/>
+      <c r="Z23" s="116"/>
       <c r="AA23" s="30"/>
       <c r="AB23" s="30"/>
       <c r="AC23" s="30"/>
     </row>
     <row r="24" ht="17.25" customHeight="1">
-      <c r="A24" s="114"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="115"/>
-      <c r="P24" s="116"/>
-      <c r="Q24" s="116"/>
-      <c r="R24" s="116"/>
-      <c r="S24" s="116"/>
-      <c r="T24" s="116"/>
-      <c r="U24" s="116"/>
-      <c r="V24" s="115"/>
-      <c r="W24" s="115"/>
-      <c r="X24" s="115"/>
-      <c r="Y24" s="115"/>
-      <c r="Z24" s="115"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="115"/>
+      <c r="G24" s="115"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="115"/>
+      <c r="K24" s="115"/>
+      <c r="L24" s="115"/>
+      <c r="M24" s="115"/>
+      <c r="N24" s="115"/>
+      <c r="O24" s="116"/>
+      <c r="P24" s="117"/>
+      <c r="Q24" s="117"/>
+      <c r="R24" s="117"/>
+      <c r="S24" s="117"/>
+      <c r="T24" s="117"/>
+      <c r="U24" s="117"/>
+      <c r="V24" s="116"/>
+      <c r="W24" s="116"/>
+      <c r="X24" s="116"/>
+      <c r="Y24" s="116"/>
+      <c r="Z24" s="116"/>
       <c r="AA24" s="30"/>
       <c r="AB24" s="30"/>
       <c r="AC24" s="30"/>
@@ -23927,7 +23930,7 @@
       <c r="P2" s="35"/>
       <c r="Q2" s="35"/>
       <c r="R2" s="35"/>
-      <c r="S2" s="117" t="s">
+      <c r="S2" s="118" t="s">
         <v>42</v>
       </c>
       <c r="Y2" s="34"/>
@@ -24024,8 +24027,8 @@
       <c r="T6" s="45"/>
       <c r="U6" s="45"/>
       <c r="V6" s="30"/>
-      <c r="W6" s="118"/>
-      <c r="X6" s="119"/>
+      <c r="W6" s="119"/>
+      <c r="X6" s="120"/>
       <c r="Y6" s="30"/>
       <c r="Z6" s="30"/>
       <c r="AA6" s="30"/>
@@ -24200,13 +24203,13 @@
       </c>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="120"/>
+      <c r="E12" s="121"/>
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
@@ -24236,11 +24239,11 @@
       <c r="A13" s="30"/>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="121"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
       <c r="K13" s="56"/>
@@ -24309,12 +24312,12 @@
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="60"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="122"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
       <c r="I15" s="60"/>
       <c r="J15" s="60"/>
       <c r="K15" s="60"/>
@@ -24600,30 +24603,30 @@
     </row>
     <row r="23" ht="16.5" customHeight="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="123"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="123"/>
-      <c r="O23" s="123"/>
-      <c r="P23" s="123"/>
-      <c r="Q23" s="123"/>
-      <c r="R23" s="123"/>
-      <c r="S23" s="123"/>
-      <c r="T23" s="123"/>
-      <c r="U23" s="123"/>
-      <c r="V23" s="123"/>
-      <c r="W23" s="123"/>
-      <c r="X23" s="123"/>
-      <c r="Y23" s="123"/>
+      <c r="B23" s="124"/>
+      <c r="C23" s="124"/>
+      <c r="D23" s="124"/>
+      <c r="E23" s="124"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="124"/>
+      <c r="H23" s="124"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="124"/>
+      <c r="K23" s="124"/>
+      <c r="L23" s="124"/>
+      <c r="M23" s="124"/>
+      <c r="N23" s="124"/>
+      <c r="O23" s="124"/>
+      <c r="P23" s="124"/>
+      <c r="Q23" s="124"/>
+      <c r="R23" s="124"/>
+      <c r="S23" s="124"/>
+      <c r="T23" s="124"/>
+      <c r="U23" s="124"/>
+      <c r="V23" s="124"/>
+      <c r="W23" s="124"/>
+      <c r="X23" s="124"/>
+      <c r="Y23" s="124"/>
       <c r="Z23" s="30"/>
       <c r="AA23" s="30"/>
       <c r="AB23" s="30"/>
@@ -33024,7 +33027,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
       <c r="N4" s="41"/>
-      <c r="O4" s="124" t="s">
+      <c r="O4" s="125" t="s">
         <v>48</v>
       </c>
       <c r="X4" s="43"/>
@@ -33196,7 +33199,7 @@
       <c r="O10" s="45"/>
       <c r="P10" s="45"/>
       <c r="Q10" s="30"/>
-      <c r="R10" s="125"/>
+      <c r="R10" s="126"/>
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
       <c r="U10" s="30"/>
@@ -33233,7 +33236,7 @@
       <c r="O11" s="30"/>
       <c r="P11" s="45"/>
       <c r="Q11" s="30"/>
-      <c r="R11" s="125"/>
+      <c r="R11" s="126"/>
       <c r="S11" s="30"/>
       <c r="T11" s="30"/>
       <c r="U11" s="30"/>
@@ -33259,7 +33262,7 @@
       </c>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="120"/>
+      <c r="E12" s="121"/>
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
@@ -33272,7 +33275,7 @@
       <c r="O12" s="30"/>
       <c r="P12" s="45"/>
       <c r="Q12" s="45"/>
-      <c r="R12" s="125"/>
+      <c r="R12" s="126"/>
       <c r="S12" s="45"/>
       <c r="T12" s="45"/>
       <c r="U12" s="45"/>
@@ -33296,10 +33299,10 @@
       <c r="B13" s="56"/>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="121"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
       <c r="K13" s="56"/>
@@ -33372,12 +33375,12 @@
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="60"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="122"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
       <c r="I15" s="60"/>
       <c r="J15" s="60"/>
       <c r="K15" s="60"/>
@@ -33486,7 +33489,7 @@
         <v>0.0</v>
       </c>
       <c r="J18" s="85"/>
-      <c r="K18" s="126"/>
+      <c r="K18" s="127"/>
       <c r="L18" s="86"/>
       <c r="M18" s="87"/>
       <c r="N18" s="85"/>
@@ -33518,7 +33521,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="92"/>
-      <c r="D19" s="127"/>
+      <c r="D19" s="128"/>
       <c r="E19" s="92"/>
       <c r="F19" s="92"/>
       <c r="G19" s="92"/>

</xml_diff>